<commit_message>
addProductwithallFields and mandatory fields code Updated
</commit_message>
<xml_diff>
--- a/TestData/OrbitScience.xlsx
+++ b/TestData/OrbitScience.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Smoke" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
   <si>
     <t>#</t>
   </si>
@@ -42,9 +42,6 @@
     <t>admin@123</t>
   </si>
   <si>
-    <t>C:\\Users\\Chaitanya\\Desktop\\Project details\\Sample images\\bencodryl-sf-500x500.jpg</t>
-  </si>
-  <si>
     <t>TC002_addSubCategory</t>
   </si>
   <si>
@@ -81,17 +78,23 @@
     <t>One time inventory</t>
   </si>
   <si>
-    <t>O</t>
-  </si>
-  <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>C:\Users\DELL\Desktop\\download (2).jpg</t>
+  </si>
+  <si>
+    <t>Paracip</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,7 +199,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -231,7 +234,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -408,31 +411,31 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="25.28515625" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="84.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -446,7 +449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -460,115 +463,115 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>

</xml_diff>